<commit_message>
Update UAT FIX POLRES
</commit_message>
<xml_diff>
--- a/UAT GISBEGAL.xlsx
+++ b/UAT GISBEGAL.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SKRIPSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD612CA-CAF1-42AF-9089-2ACB188D84A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623B7DAA-E789-4B0F-BD11-2B9C4D5CF260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{335E6562-EAC7-450D-8F68-8E81A96047F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{335E6562-EAC7-450D-8F68-8E81A96047F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Umum" sheetId="2" r:id="rId2"/>
+    <sheet name="POLRES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="131">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -380,6 +381,45 @@
   </si>
   <si>
     <t>Seberapa setuju Anda dengan pernyataan bahwa  secara keseluruhan website ini bermanfaat</t>
+  </si>
+  <si>
+    <t>Seberapa setuju Anda dengan pernyataan bahwa  tombol-tombol seperti “Cek Daerahmu”, “Curas”, atau “Curanmor”, dll mudah ditemukan dan dimengerti fungsinya?</t>
+  </si>
+  <si>
+    <t>Seberapa mudah Anda memahami struktur menu di dashboard admin (seperti menu Kecamatan, Klaster, Curas &amp; Curanmor, Hasil Pemetaan, dll)?</t>
+  </si>
+  <si>
+    <t>Seberapa jelas dan mudah dipahami tampilan dari ringkasan data data utama yang ada pada halaman dashboard</t>
+  </si>
+  <si>
+    <t>Seberapa mudah Anda bisa memahami data seperti kecamatan dan klaster pada masing masing halaman tersebut</t>
+  </si>
+  <si>
+    <t>Seberapa mudah Anda bisa memahami data Curas dan Curanmor pada masing masing halaman tersebut</t>
+  </si>
+  <si>
+    <t>Seberapa mudah Anda bisa memahami penambahan data Curas dan Curanmor pada halaman detail</t>
+  </si>
+  <si>
+    <t>Seberapa setuju Anda jika proses untuk menambah, mengedit, atau menghapus data (CRUD) untuk data Curas dan Curanmor sudah cukup mudah dilakukan?</t>
+  </si>
+  <si>
+    <t>Seberapa setuju Anda jika validasi atau notifikasi setelah menginput atau mengubah data sudah cukup membantu (misalnya: pesan sukses dan gagal)</t>
+  </si>
+  <si>
+    <t>Seberapa setuju Anda jika proses untuk menambah, mengedit, atau menghapus data (CRUD) untuk data kecamatan dan klaster sudah cukup mudah dilakukan?</t>
+  </si>
+  <si>
+    <t>Seberapa mudah Anda dalam memahami detail perhitungan k-means yang ada ?</t>
+  </si>
+  <si>
+    <t>C. Pengujian Secara Keseluruhan</t>
+  </si>
+  <si>
+    <t>A. Pengujian Untuk Akses Pengguna dan Admin</t>
+  </si>
+  <si>
+    <t>B. Pengujian Untuk Akses Admin</t>
   </si>
 </sst>
 </file>
@@ -593,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -621,27 +661,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -651,6 +691,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -717,12 +763,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -731,6 +771,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1117,33 +1169,33 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -1957,73 +2009,73 @@
       <c r="B85" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
     </row>
     <row r="86" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="12">
+      <c r="A86" s="13">
         <v>2</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D86" s="19"/>
-      <c r="E86" s="19"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
       <c r="I86" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
+      <c r="A87" s="13"/>
       <c r="B87" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
     </row>
     <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
+      <c r="A88" s="13"/>
       <c r="B88" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
     </row>
     <row r="89" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
+      <c r="A89" s="13"/>
       <c r="B89" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
     </row>
     <row r="90" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
+      <c r="A90" s="13"/>
       <c r="B90" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
+      <c r="A91" s="13"/>
       <c r="B91" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="18"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="18"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
     </row>
     <row r="92" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="12">
+      <c r="A92" s="13">
         <v>3</v>
       </c>
       <c r="B92" s="15" t="s">
@@ -2034,47 +2086,47 @@
       <c r="E92" s="15"/>
     </row>
     <row r="93" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
+      <c r="A93" s="13"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
     </row>
     <row r="94" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="12">
+      <c r="A94" s="13">
         <v>4</v>
       </c>
-      <c r="B94" s="18" t="s">
+      <c r="B94" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="18"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
     </row>
     <row r="95" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="12"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
+      <c r="A95" s="13"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
     </row>
     <row r="96" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="12">
+      <c r="A96" s="13">
         <v>5</v>
       </c>
-      <c r="B96" s="19" t="s">
+      <c r="B96" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
     </row>
     <row r="97" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
+      <c r="A97" s="13"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
     </row>
     <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
@@ -2099,12 +2151,25 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B94:E94"/>
-    <mergeCell ref="B95:E95"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B97:E97"/>
-    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A73:E73"/>
+    <mergeCell ref="A74:E74"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A84:E84"/>
     <mergeCell ref="C85:E85"/>
     <mergeCell ref="B92:E92"/>
@@ -2117,25 +2182,12 @@
     <mergeCell ref="C90:E90"/>
     <mergeCell ref="C91:E91"/>
     <mergeCell ref="A86:A91"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A73:E73"/>
-    <mergeCell ref="A74:E74"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B94:E94"/>
+    <mergeCell ref="B95:E95"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B97:E97"/>
+    <mergeCell ref="A96:A97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2146,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5AA470-3FE3-40EB-A7B3-B029ED87CB95}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,27 +2211,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="4">
         <v>1</v>
       </c>
@@ -2200,12 +2252,12 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -2216,12 +2268,12 @@
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -2232,12 +2284,12 @@
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -2248,12 +2300,12 @@
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -2264,12 +2316,12 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2280,12 +2332,12 @@
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -2296,12 +2348,12 @@
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -2312,12 +2364,12 @@
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -2328,12 +2380,12 @@
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2344,12 +2396,12 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -2360,12 +2412,12 @@
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -2376,12 +2428,12 @@
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -2392,12 +2444,12 @@
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -2408,12 +2460,12 @@
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
@@ -2440,12 +2492,12 @@
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
@@ -2453,7 +2505,7 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="45">
+      <c r="A19" s="24">
         <v>17</v>
       </c>
       <c r="B19" s="20" t="s">
@@ -2462,84 +2514,84 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="28"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="28"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="28"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="30"/>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="28"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="28"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
+      <c r="A25" s="13">
         <v>18</v>
       </c>
       <c r="B25" s="15" t="s">
@@ -2548,139 +2600,116 @@
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="30"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="28"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="30"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44">
+      <c r="A27" s="46">
         <v>19</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="28"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="30"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="47"/>
       <c r="C28" s="48"/>
       <c r="D28" s="48"/>
       <c r="E28" s="49"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
+      <c r="A29" s="13">
         <v>20</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="28"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="28"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="A31" s="13">
         <v>21</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="28"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="31"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="33"/>
     </row>
     <row r="37" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H37" s="10"/>
     </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H39" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="B17:E17"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F19:J32"/>
@@ -2696,6 +2725,787 @@
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220A1F9A-91CC-43D1-87ED-EB159AD0E01C}">
+  <dimension ref="A1:J44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="50"/>
+    <col min="2" max="2" width="21.28515625" style="50" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="50"/>
+    <col min="5" max="5" width="27.28515625" style="50" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="50"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+    </row>
+    <row r="6" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+    </row>
+    <row r="7" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+    </row>
+    <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+    </row>
+    <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+    </row>
+    <row r="11" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+    </row>
+    <row r="12" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>9</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+    </row>
+    <row r="13" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+    </row>
+    <row r="14" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+    </row>
+    <row r="16" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+    </row>
+    <row r="17" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>3</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+    </row>
+    <row r="18" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>4</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+    </row>
+    <row r="19" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>5</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+    </row>
+    <row r="20" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>6</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+    </row>
+    <row r="21" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>7</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+    </row>
+    <row r="22" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>8</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+    </row>
+    <row r="23" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>9</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+    </row>
+    <row r="24" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>2</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>3</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>4</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>5</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>6</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>7</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <v>8</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <v>9</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>10</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>11</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>12</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
+        <v>13</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="51">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="B44:J44"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="C36:J36"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>